<commit_message>
Add business-exception-dealing Refactor MainChart Add LoadList Add ReadConfig Add WriteList Add MainChart-ScreenShot in README
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -54,6 +54,32 @@
         <charset val="128"/>
       </rPr>
       <t xml:space="preserve">対象画像ファイルの情報が記入されるスプレッドシートのパス。</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">image-list-sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheet1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">OCR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">対象画像ファイルの情報が記入されるスプレッドシートのシート名。</t>
     </r>
   </si>
   <si>
@@ -1057,10 +1083,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1100,7 +1126,7 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1115,80 +1141,80 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4" t="n">
-        <v>1920</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="n">
-        <v>1080</v>
+        <v>1920</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>1400</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>17</v>
+        <v>1080</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="8" t="n">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>1400</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="8" t="n">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="8" t="n">
+        <v>500</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="8" t="n">
         <v>160</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1197,31 +1223,31 @@
         <v>27</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1240,32 +1266,32 @@
       <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="8" t="n">
+      <c r="B16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="8" t="n">
         <v>312</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1273,22 +1299,33 @@
       <c r="A19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="8" t="n">
-        <v>3</v>
+      <c r="B19" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B20" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="8" t="n">
         <v>1.5</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>48</v>
+      <c r="C21" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>